<commit_message>
20220325 - Massive Update: Re-Architectured
</commit_message>
<xml_diff>
--- a/tdatlib/archive/market/classify/__ETF.xlsx
+++ b/tdatlib/archive/market/classify/__ETF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5707692dd86f11a/프로그래밍/Back-End/tdatlib/tdatlib/archive/market/classify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="13_ncr:1_{95B76DB8-6987-4161-B515-97E22888F8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04C2FE0C-95F4-478A-8BDA-B775698C73E6}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="13_ncr:1_{95B76DB8-6987-4161-B515-97E22888F8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174C1117-276A-4E19-AE5C-F93373BF5A7E}"/>
   <bookViews>
     <workbookView xWindow="2715" yWindow="690" windowWidth="15480" windowHeight="11385" xr2:uid="{F3E23080-6921-44B6-B0A9-6FAFD4DE058E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$525</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$527</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="613">
   <si>
     <t>종목코드</t>
   </si>
@@ -1952,6 +1952,24 @@
   </si>
   <si>
     <t>히어로즈 단기채권ESG액티브</t>
+  </si>
+  <si>
+    <t>KODEX 차이나2차전지MSCI(합성)</t>
+  </si>
+  <si>
+    <t>해외</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KODEX 미국클린에너지나스닥</t>
+  </si>
+  <si>
+    <t>미국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2349,11 +2367,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3E65B9-4AFB-4959-9CD3-28669B32D629}">
-  <dimension ref="A1:D548"/>
+  <dimension ref="A1:D550"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C363" sqref="C363:D363"/>
+      <pane ySplit="1" topLeftCell="A407" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B426" sqref="B426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8286,38 +8304,38 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424">
-        <v>381180</v>
+        <v>419430</v>
       </c>
       <c r="B424" t="s">
-        <v>391</v>
+        <v>608</v>
       </c>
       <c r="C424" t="s">
-        <v>496</v>
+        <v>609</v>
       </c>
       <c r="D424" t="s">
-        <v>487</v>
+        <v>610</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>381170</v>
+        <v>419420</v>
       </c>
       <c r="B425" t="s">
-        <v>392</v>
+        <v>611</v>
       </c>
       <c r="C425" t="s">
-        <v>496</v>
+        <v>609</v>
       </c>
       <c r="D425" t="s">
-        <v>487</v>
+        <v>612</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A426">
-        <v>379810</v>
+        <v>381180</v>
       </c>
       <c r="B426" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C426" t="s">
         <v>496</v>
@@ -8328,10 +8346,10 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427">
-        <v>379800</v>
+        <v>381170</v>
       </c>
       <c r="B427" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C427" t="s">
         <v>496</v>
@@ -8342,164 +8360,164 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428">
-        <v>150460</v>
+        <v>379810</v>
       </c>
       <c r="B428" t="s">
-        <v>230</v>
+        <v>393</v>
       </c>
       <c r="C428" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D428" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429">
-        <v>371130</v>
+        <v>379800</v>
       </c>
       <c r="B429" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C429" t="s">
         <v>496</v>
       </c>
       <c r="D429" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430">
-        <v>379790</v>
+        <v>150460</v>
       </c>
       <c r="B430" t="s">
-        <v>396</v>
+        <v>230</v>
       </c>
       <c r="C430" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="D430" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A431">
-        <v>400570</v>
+        <v>371130</v>
       </c>
       <c r="B431" t="s">
-        <v>544</v>
+        <v>395</v>
       </c>
       <c r="C431" t="s">
         <v>496</v>
       </c>
       <c r="D431" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A432">
-        <v>143850</v>
+        <v>379790</v>
       </c>
       <c r="B432" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C432" t="s">
         <v>496</v>
       </c>
       <c r="D432" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>236350</v>
+        <v>400570</v>
       </c>
       <c r="B433" t="s">
-        <v>398</v>
+        <v>544</v>
       </c>
       <c r="C433" t="s">
         <v>496</v>
       </c>
       <c r="D433" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A434">
-        <v>276650</v>
+        <v>143850</v>
       </c>
       <c r="B434" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C434" t="s">
         <v>496</v>
       </c>
       <c r="D434" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435">
-        <v>276000</v>
+        <v>236350</v>
       </c>
       <c r="B435" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C435" t="s">
         <v>496</v>
       </c>
       <c r="D435" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436">
-        <v>133690</v>
+        <v>276650</v>
       </c>
       <c r="B436" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C436" t="s">
         <v>496</v>
       </c>
       <c r="D436" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>418660</v>
+        <v>276000</v>
       </c>
       <c r="B437" t="s">
-        <v>602</v>
+        <v>400</v>
       </c>
       <c r="C437" t="s">
         <v>496</v>
       </c>
       <c r="D437" t="s">
-        <v>605</v>
+        <v>486</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438">
-        <v>418670</v>
+        <v>133690</v>
       </c>
       <c r="B438" t="s">
-        <v>603</v>
+        <v>401</v>
       </c>
       <c r="C438" t="s">
         <v>496</v>
       </c>
       <c r="D438" t="s">
-        <v>606</v>
+        <v>487</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439">
-        <v>419170</v>
+        <v>418660</v>
       </c>
       <c r="B439" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C439" t="s">
         <v>496</v>
@@ -8510,52 +8528,52 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A440">
-        <v>275980</v>
+        <v>418670</v>
       </c>
       <c r="B440" t="s">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C440" t="s">
         <v>496</v>
       </c>
       <c r="D440" t="s">
-        <v>486</v>
+        <v>606</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441">
-        <v>373790</v>
+        <v>419170</v>
       </c>
       <c r="B441" t="s">
-        <v>403</v>
+        <v>604</v>
       </c>
       <c r="C441" t="s">
         <v>496</v>
       </c>
       <c r="D441" t="s">
-        <v>487</v>
+        <v>605</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442">
-        <v>373530</v>
+        <v>275980</v>
       </c>
       <c r="B442" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C442" t="s">
         <v>496</v>
       </c>
       <c r="D442" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443">
-        <v>287180</v>
+        <v>373790</v>
       </c>
       <c r="B443" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C443" t="s">
         <v>496</v>
@@ -8566,38 +8584,38 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444">
-        <v>372330</v>
+        <v>373530</v>
       </c>
       <c r="B444" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C444" t="s">
         <v>496</v>
       </c>
       <c r="D444" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>371870</v>
+        <v>287180</v>
       </c>
       <c r="B445" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C445" t="s">
         <v>496</v>
       </c>
       <c r="D445" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446">
-        <v>371470</v>
+        <v>372330</v>
       </c>
       <c r="B446" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C446" t="s">
         <v>496</v>
@@ -8608,10 +8626,10 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447">
-        <v>371460</v>
+        <v>371870</v>
       </c>
       <c r="B447" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C447" t="s">
         <v>496</v>
@@ -8622,10 +8640,10 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448">
-        <v>371160</v>
+        <v>371470</v>
       </c>
       <c r="B448" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C448" t="s">
         <v>496</v>
@@ -8636,248 +8654,248 @@
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>379780</v>
+        <v>371460</v>
       </c>
       <c r="B449" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C449" t="s">
         <v>496</v>
       </c>
       <c r="D449" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450">
-        <v>309230</v>
+        <v>371160</v>
       </c>
       <c r="B450" t="s">
-        <v>157</v>
+        <v>410</v>
       </c>
       <c r="C450" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D450" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451">
-        <v>245350</v>
+        <v>379780</v>
       </c>
       <c r="B451" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C451" t="s">
         <v>496</v>
       </c>
       <c r="D451" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452">
-        <v>360750</v>
+        <v>309230</v>
       </c>
       <c r="B452" t="s">
-        <v>414</v>
+        <v>157</v>
       </c>
       <c r="C452" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D452" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453">
-        <v>399110</v>
+        <v>245350</v>
       </c>
       <c r="B453" t="s">
-        <v>547</v>
+        <v>412</v>
       </c>
       <c r="C453" t="s">
         <v>496</v>
       </c>
       <c r="D453" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A454">
-        <v>400580</v>
+        <v>360750</v>
       </c>
       <c r="B454" t="s">
-        <v>548</v>
+        <v>414</v>
       </c>
       <c r="C454" t="s">
         <v>496</v>
       </c>
       <c r="D454" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>400590</v>
+        <v>399110</v>
       </c>
       <c r="B455" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C455" t="s">
         <v>496</v>
       </c>
       <c r="D455" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A456">
-        <v>401590</v>
+        <v>400580</v>
       </c>
       <c r="B456" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C456" t="s">
         <v>496</v>
       </c>
       <c r="D456" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>195930</v>
+        <v>400590</v>
       </c>
       <c r="B457" t="s">
-        <v>415</v>
+        <v>549</v>
       </c>
       <c r="C457" t="s">
         <v>496</v>
       </c>
       <c r="D457" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A458">
-        <v>195970</v>
+        <v>401590</v>
       </c>
       <c r="B458" t="s">
-        <v>416</v>
+        <v>550</v>
       </c>
       <c r="C458" t="s">
         <v>496</v>
       </c>
       <c r="D458" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A459">
-        <v>195980</v>
+        <v>195930</v>
       </c>
       <c r="B459" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C459" t="s">
         <v>496</v>
       </c>
       <c r="D459" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A460">
-        <v>196030</v>
+        <v>195970</v>
       </c>
       <c r="B460" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C460" t="s">
         <v>496</v>
       </c>
       <c r="D460" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>277540</v>
+        <v>195980</v>
       </c>
       <c r="B461" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C461" t="s">
         <v>496</v>
       </c>
       <c r="D461" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462">
-        <v>399580</v>
+        <v>196030</v>
       </c>
       <c r="B462" t="s">
-        <v>556</v>
+        <v>418</v>
       </c>
       <c r="C462" t="s">
         <v>496</v>
       </c>
       <c r="D462" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463">
-        <v>200030</v>
+        <v>277540</v>
       </c>
       <c r="B463" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C463" t="s">
         <v>496</v>
       </c>
       <c r="D463" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A464">
-        <v>402970</v>
+        <v>399580</v>
       </c>
       <c r="B464" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C464" t="s">
         <v>496</v>
       </c>
       <c r="D464" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465">
-        <v>200250</v>
+        <v>200030</v>
       </c>
       <c r="B465" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C465" t="s">
         <v>496</v>
       </c>
       <c r="D465" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A466">
-        <v>203780</v>
+        <v>402970</v>
       </c>
       <c r="B466" t="s">
-        <v>423</v>
+        <v>557</v>
       </c>
       <c r="C466" t="s">
         <v>496</v>
@@ -8888,38 +8906,38 @@
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A467">
-        <v>204450</v>
+        <v>200250</v>
       </c>
       <c r="B467" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C467" t="s">
         <v>496</v>
       </c>
       <c r="D467" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A468">
-        <v>217780</v>
+        <v>203780</v>
       </c>
       <c r="B468" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C468" t="s">
         <v>496</v>
       </c>
       <c r="D468" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A469">
-        <v>204480</v>
+        <v>204450</v>
       </c>
       <c r="B469" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C469" t="s">
         <v>496</v>
@@ -8930,108 +8948,108 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A470">
-        <v>205720</v>
+        <v>217780</v>
       </c>
       <c r="B470" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C470" t="s">
         <v>496</v>
       </c>
       <c r="D470" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>208470</v>
+        <v>204480</v>
       </c>
       <c r="B471" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C471" t="s">
         <v>496</v>
       </c>
       <c r="D471" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A472">
-        <v>261920</v>
+        <v>205720</v>
       </c>
       <c r="B472" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C472" t="s">
         <v>496</v>
       </c>
       <c r="D472" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>265690</v>
+        <v>208470</v>
       </c>
       <c r="B473" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C473" t="s">
         <v>496</v>
       </c>
       <c r="D473" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A474">
-        <v>314250</v>
+        <v>261920</v>
       </c>
       <c r="B474" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C474" t="s">
         <v>496</v>
       </c>
       <c r="D474" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A475">
-        <v>245360</v>
+        <v>265690</v>
       </c>
       <c r="B475" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C475" t="s">
         <v>496</v>
       </c>
       <c r="D475" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A476">
-        <v>310080</v>
+        <v>314250</v>
       </c>
       <c r="B476" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C476" t="s">
         <v>496</v>
       </c>
       <c r="D476" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A477">
-        <v>250730</v>
+        <v>245360</v>
       </c>
       <c r="B477" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C477" t="s">
         <v>496</v>
@@ -9042,248 +9060,248 @@
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A478">
-        <v>213630</v>
+        <v>310080</v>
       </c>
       <c r="B478" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C478" t="s">
         <v>496</v>
       </c>
       <c r="D478" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>245710</v>
+        <v>250730</v>
       </c>
       <c r="B479" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C479" t="s">
         <v>496</v>
       </c>
       <c r="D479" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A480">
-        <v>248270</v>
+        <v>213630</v>
       </c>
       <c r="B480" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C480" t="s">
         <v>496</v>
       </c>
       <c r="D480" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>195920</v>
+        <v>245710</v>
       </c>
       <c r="B481" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C481" t="s">
         <v>496</v>
       </c>
       <c r="D481" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>101280</v>
+        <v>248270</v>
       </c>
       <c r="B482" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C482" t="s">
         <v>496</v>
       </c>
       <c r="D482" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A483">
-        <v>192090</v>
+        <v>195920</v>
       </c>
       <c r="B483" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C483" t="s">
         <v>496</v>
       </c>
       <c r="D483" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>218420</v>
+        <v>101280</v>
       </c>
       <c r="B484" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C484" t="s">
         <v>496</v>
       </c>
       <c r="D484" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>360200</v>
+        <v>192090</v>
       </c>
       <c r="B485" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C485" t="s">
         <v>496</v>
       </c>
       <c r="D485" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A486">
-        <v>269530</v>
+        <v>218420</v>
       </c>
       <c r="B486" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C486" t="s">
         <v>496</v>
       </c>
       <c r="D486" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>269420</v>
+        <v>360200</v>
       </c>
       <c r="B487" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C487" t="s">
         <v>496</v>
       </c>
       <c r="D487" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A488">
-        <v>168580</v>
+        <v>269530</v>
       </c>
       <c r="B488" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C488" t="s">
         <v>496</v>
       </c>
       <c r="D488" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>319870</v>
+        <v>269420</v>
       </c>
       <c r="B489" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="C489" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D489" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>248260</v>
+        <v>168580</v>
       </c>
       <c r="B490" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C490" t="s">
         <v>496</v>
       </c>
       <c r="D490" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>169950</v>
+        <v>319870</v>
       </c>
       <c r="B491" t="s">
-        <v>449</v>
+        <v>166</v>
       </c>
       <c r="C491" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="D491" t="s">
-        <v>483</v>
+        <v>502</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>354350</v>
+        <v>248260</v>
       </c>
       <c r="B492" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C492" t="s">
         <v>496</v>
       </c>
       <c r="D492" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>269370</v>
+        <v>169950</v>
       </c>
       <c r="B493" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C493" t="s">
         <v>496</v>
       </c>
       <c r="D493" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A494">
-        <v>225060</v>
+        <v>354350</v>
       </c>
       <c r="B494" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C494" t="s">
         <v>496</v>
       </c>
       <c r="D494" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>298770</v>
+        <v>269370</v>
       </c>
       <c r="B495" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C495" t="s">
         <v>496</v>
@@ -9294,52 +9312,52 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A496">
-        <v>174360</v>
+        <v>225060</v>
       </c>
       <c r="B496" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C496" t="s">
         <v>496</v>
       </c>
       <c r="D496" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A497">
-        <v>269540</v>
+        <v>298770</v>
       </c>
       <c r="B497" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C497" t="s">
         <v>496</v>
       </c>
       <c r="D497" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>225050</v>
+        <v>174360</v>
       </c>
       <c r="B498" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C498" t="s">
         <v>496</v>
       </c>
       <c r="D498" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>225030</v>
+        <v>269540</v>
       </c>
       <c r="B499" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C499" t="s">
         <v>496</v>
@@ -9350,52 +9368,52 @@
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A500">
-        <v>220130</v>
+        <v>225050</v>
       </c>
       <c r="B500" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C500" t="s">
         <v>496</v>
       </c>
       <c r="D500" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>219900</v>
+        <v>225030</v>
       </c>
       <c r="B501" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C501" t="s">
         <v>496</v>
       </c>
       <c r="D501" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>185680</v>
+        <v>220130</v>
       </c>
       <c r="B502" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C502" t="s">
         <v>496</v>
       </c>
       <c r="D502" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>99140</v>
+        <v>219900</v>
       </c>
       <c r="B503" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C503" t="s">
         <v>496</v>
@@ -9406,66 +9424,66 @@
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>189400</v>
+        <v>185680</v>
       </c>
       <c r="B504" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C504" t="s">
         <v>496</v>
       </c>
       <c r="D504" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A505">
-        <v>105010</v>
+        <v>99140</v>
       </c>
       <c r="B505" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C505" t="s">
         <v>496</v>
       </c>
       <c r="D505" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>219480</v>
+        <v>189400</v>
       </c>
       <c r="B506" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C506" t="s">
         <v>496</v>
       </c>
       <c r="D506" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A507">
-        <v>304940</v>
+        <v>105010</v>
       </c>
       <c r="B507" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C507" t="s">
         <v>496</v>
       </c>
       <c r="D507" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>225040</v>
+        <v>219480</v>
       </c>
       <c r="B508" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C508" t="s">
         <v>496</v>
@@ -9476,10 +9494,10 @@
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>219390</v>
+        <v>304940</v>
       </c>
       <c r="B509" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C509" t="s">
         <v>496</v>
@@ -9490,13 +9508,13 @@
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>138230</v>
+        <v>225040</v>
       </c>
       <c r="B510" t="s">
-        <v>272</v>
+        <v>470</v>
       </c>
       <c r="C510" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D510" t="s">
         <v>490</v>
@@ -9504,13 +9522,13 @@
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>261110</v>
+        <v>219390</v>
       </c>
       <c r="B511" t="s">
-        <v>274</v>
+        <v>471</v>
       </c>
       <c r="C511" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D511" t="s">
         <v>490</v>
@@ -9518,24 +9536,24 @@
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A512">
-        <v>292560</v>
+        <v>138230</v>
       </c>
       <c r="B512" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C512" t="s">
         <v>497</v>
       </c>
       <c r="D512" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A513">
-        <v>261120</v>
+        <v>261110</v>
       </c>
       <c r="B513" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C513" t="s">
         <v>497</v>
@@ -9546,10 +9564,10 @@
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A514">
-        <v>352540</v>
+        <v>292560</v>
       </c>
       <c r="B514" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C514" t="s">
         <v>497</v>
@@ -9560,10 +9578,10 @@
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>354240</v>
+        <v>261120</v>
       </c>
       <c r="B515" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C515" t="s">
         <v>497</v>
@@ -9574,24 +9592,24 @@
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>352560</v>
+        <v>352540</v>
       </c>
       <c r="B516" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C516" t="s">
         <v>497</v>
       </c>
       <c r="D516" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A517">
-        <v>261270</v>
+        <v>354240</v>
       </c>
       <c r="B517" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C517" t="s">
         <v>497</v>
@@ -9602,10 +9620,10 @@
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A518">
-        <v>182480</v>
+        <v>352560</v>
       </c>
       <c r="B518" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C518" t="s">
         <v>497</v>
@@ -9616,10 +9634,10 @@
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A519">
-        <v>261260</v>
+        <v>261270</v>
       </c>
       <c r="B519" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C519" t="s">
         <v>497</v>
@@ -9630,10 +9648,10 @@
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A520">
-        <v>139660</v>
+        <v>182480</v>
       </c>
       <c r="B520" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C520" t="s">
         <v>497</v>
@@ -9644,10 +9662,10 @@
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A521">
-        <v>261250</v>
+        <v>261260</v>
       </c>
       <c r="B521" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C521" t="s">
         <v>497</v>
@@ -9658,24 +9676,24 @@
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A522">
-        <v>375270</v>
+        <v>139660</v>
       </c>
       <c r="B522" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C522" t="s">
         <v>497</v>
       </c>
       <c r="D522" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A523">
-        <v>181480</v>
+        <v>261250</v>
       </c>
       <c r="B523" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C523" t="s">
         <v>497</v>
@@ -9686,24 +9704,24 @@
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A524">
-        <v>316300</v>
+        <v>375270</v>
       </c>
       <c r="B524" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C524" t="s">
         <v>497</v>
       </c>
       <c r="D524" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A525">
-        <v>261240</v>
+        <v>181480</v>
       </c>
       <c r="B525" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C525" t="s">
         <v>497</v>
@@ -9714,24 +9732,24 @@
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A526">
-        <v>390390</v>
+        <v>316300</v>
       </c>
       <c r="B526" t="s">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="C526" t="s">
         <v>497</v>
       </c>
       <c r="D526" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A527">
-        <v>390400</v>
+        <v>261240</v>
       </c>
       <c r="B527" t="s">
-        <v>511</v>
+        <v>301</v>
       </c>
       <c r="C527" t="s">
         <v>497</v>
@@ -9742,38 +9760,38 @@
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A528">
-        <v>394670</v>
+        <v>390390</v>
       </c>
       <c r="B528" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C528" t="s">
         <v>497</v>
       </c>
       <c r="D528" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A529">
-        <v>394660</v>
+        <v>390400</v>
       </c>
       <c r="B529" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C529" t="s">
         <v>497</v>
       </c>
       <c r="D529" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A530">
-        <v>394350</v>
+        <v>394670</v>
       </c>
       <c r="B530" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C530" t="s">
         <v>497</v>
@@ -9784,10 +9802,10 @@
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A531">
-        <v>394340</v>
+        <v>394660</v>
       </c>
       <c r="B531" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C531" t="s">
         <v>497</v>
@@ -9798,206 +9816,206 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A532">
-        <v>396510</v>
+        <v>394350</v>
       </c>
       <c r="B532" t="s">
-        <v>538</v>
+        <v>514</v>
       </c>
       <c r="C532" t="s">
         <v>497</v>
       </c>
       <c r="D532" t="s">
-        <v>542</v>
+        <v>486</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A533">
-        <v>396520</v>
+        <v>394340</v>
       </c>
       <c r="B533" t="s">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="C533" t="s">
         <v>497</v>
       </c>
       <c r="D533" t="s">
-        <v>542</v>
+        <v>486</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A534">
-        <v>391600</v>
+        <v>396510</v>
       </c>
       <c r="B534" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C534" t="s">
         <v>497</v>
       </c>
       <c r="D534" t="s">
-        <v>490</v>
+        <v>542</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A535">
-        <v>391590</v>
+        <v>396520</v>
       </c>
       <c r="B535" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C535" t="s">
         <v>497</v>
       </c>
       <c r="D535" t="s">
-        <v>490</v>
+        <v>542</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A536">
-        <v>412770</v>
+        <v>391600</v>
       </c>
       <c r="B536" t="s">
-        <v>570</v>
+        <v>540</v>
       </c>
       <c r="C536" t="s">
         <v>497</v>
       </c>
       <c r="D536" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A537">
-        <v>411420</v>
+        <v>391590</v>
       </c>
       <c r="B537" t="s">
-        <v>571</v>
+        <v>541</v>
       </c>
       <c r="C537" t="s">
         <v>497</v>
       </c>
       <c r="D537" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A538">
-        <v>409820</v>
+        <v>412770</v>
       </c>
       <c r="B538" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C538" t="s">
-        <v>577</v>
+        <v>497</v>
       </c>
       <c r="D538" t="s">
-        <v>580</v>
+        <v>486</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A539">
-        <v>409810</v>
+        <v>411420</v>
       </c>
       <c r="B539" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C539" t="s">
-        <v>577</v>
+        <v>497</v>
       </c>
       <c r="D539" t="s">
-        <v>580</v>
+        <v>486</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A540">
-        <v>411050</v>
+        <v>409820</v>
       </c>
       <c r="B540" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C540" t="s">
         <v>577</v>
       </c>
       <c r="D540" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A541">
-        <v>411720</v>
+        <v>409810</v>
       </c>
       <c r="B541" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C541" t="s">
         <v>577</v>
       </c>
       <c r="D541" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A542">
-        <v>411860</v>
+        <v>411050</v>
       </c>
       <c r="B542" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C542" t="s">
         <v>577</v>
       </c>
       <c r="D542" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A543">
-        <v>413220</v>
+        <v>411720</v>
       </c>
       <c r="B543" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="C543" t="s">
         <v>577</v>
       </c>
       <c r="D543" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A544">
-        <v>414780</v>
+        <v>411860</v>
       </c>
       <c r="B544" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="C544" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="D544" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A545">
-        <v>415340</v>
+        <v>413220</v>
       </c>
       <c r="B545" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="C545" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="D545" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A546">
-        <v>416090</v>
+        <v>414780</v>
       </c>
       <c r="B546" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C546" t="s">
         <v>595</v>
@@ -10008,10 +10026,10 @@
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A547">
-        <v>415760</v>
+        <v>415340</v>
       </c>
       <c r="B547" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C547" t="s">
         <v>595</v>
@@ -10022,15 +10040,43 @@
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A548">
-        <v>415920</v>
+        <v>416090</v>
       </c>
       <c r="B548" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C548" t="s">
         <v>595</v>
       </c>
       <c r="D548" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A549">
+        <v>415760</v>
+      </c>
+      <c r="B549" t="s">
+        <v>593</v>
+      </c>
+      <c r="C549" t="s">
+        <v>595</v>
+      </c>
+      <c r="D549" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A550">
+        <v>415920</v>
+      </c>
+      <c r="B550" t="s">
+        <v>594</v>
+      </c>
+      <c r="C550" t="s">
+        <v>595</v>
+      </c>
+      <c r="D550" t="s">
         <v>597</v>
       </c>
     </row>

</xml_diff>